<commit_message>
final update to assumptions doc
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master_v2.xlsx
+++ b/app/data/wto_proposal_settings_master_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kat/Github/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B26849-4BD6-8B45-A1E7-D6EBD2F0E10C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406A8C3F-8E64-1A40-A7BB-6C2E9A8620C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="11060" windowWidth="32940" windowHeight="12500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38260" yWindow="2000" windowWidth="32940" windowHeight="12500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="449">
   <si>
     <t>proposal</t>
   </si>
@@ -1402,6 +1402,30 @@
     <t>&lt;ol&gt;&lt;li&gt;As written, this text would prohibit all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. (2019) unless a Member can demonstrate that measures are implemented to maintain stocks at a biologically sustainable level. It is unclear how many Members would be able to satisfy this sustainability criteria, and thus we assume that such an exemption could only be acquired by vessels fulfilling our management criteria. We note that this may still be a conservative interpretation of this text because our management criteria are determined based on the location in which the fishing takes place, as opposed to by the flag- or subsidizing Member state.&lt;/li&gt;&lt;li&gt;We assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. (2019) are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas and/or in the EEZs of another coastal state to be prohibited.&lt;/li&gt;&lt;/ol&gt;</t>
   </si>
   <si>
+    <t>NOTE: No guidance is provided as to potential values for X%, Y%, and Z%. 10%, 20% and 30% were chosen. The exemption for developing countries for fishing within their territorial waters is not modeled here.</t>
+  </si>
+  <si>
+    <t>Subsidies granted by developing and LDC Members shall be allowed for small-scale fishing within their own territorial waters. As written, this exemption might only apply with a transition period, but for the purposes of modeling we assume it to apply indefinitely.</t>
+  </si>
+  <si>
+    <t>Subsidies granted by developing and LDC Members shall be allowed for fishing within their own territorial waters. As written, this exemption might only apply with a transition period, but for the purposes of modeling we assume it to apply indefinitely.</t>
+  </si>
+  <si>
+    <t>Subsidies granted by LDCs shall be allowed, and subsidies granted by developing countries shall be allowed for fishing in their territorial seas, or for fishing in their EEZs and high seas unless any of the following conditions are met for three consecutive years (2016-2018): a) GNI per capita is greater than US $5000 (constant 2010 US$), b) they engage in distant water fishing, or c) the contribution from Agriculture, Forestry and Fishing to their national GDP (World Bank) is greater than 10%. As written, this exemption might only apply with a transition period, but for the purposes of modeling we assume it to apply indefinitely.</t>
+  </si>
+  <si>
+    <t>Facilitator's text - Overfished [Objective Definition]</t>
+  </si>
+  <si>
+    <t>Facilitator's text - Overfished [Relevant Authorities]</t>
+  </si>
+  <si>
+    <t>Chad on behalf of the Least Developed Countries (LDC) Group</t>
+  </si>
+  <si>
+    <t>Ecuador, Argentina, and Chile</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -1418,32 +1442,11 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> 10/22/22 - Updated text. 7/13/21 - Updated text again. 6/8/21 - Updated text. 5/25/21 - NEW. </t>
+      <t xml:space="preserve"> 10/22/22 - Updated text. 10/19/21 - Added for Pew's reference.</t>
     </r>
   </si>
   <si>
-    <t>NOTE: No guidance is provided as to potential values for X%, Y%, and Z%. 10%, 20% and 30% were chosen. The exemption for developing countries for fishing within their territorial waters is not modeled here.</t>
-  </si>
-  <si>
-    <t>Subsidies granted by developing and LDC Members shall be allowed for small-scale fishing within their own territorial waters. As written, this exemption might only apply with a transition period, but for the purposes of modeling we assume it to apply indefinitely.</t>
-  </si>
-  <si>
-    <t>Subsidies granted by developing and LDC Members shall be allowed for fishing within their own territorial waters. As written, this exemption might only apply with a transition period, but for the purposes of modeling we assume it to apply indefinitely.</t>
-  </si>
-  <si>
-    <t>Subsidies granted by LDCs shall be allowed, and subsidies granted by developing countries shall be allowed for fishing in their territorial seas, or for fishing in their EEZs and high seas unless any of the following conditions are met for three consecutive years (2016-2018): a) GNI per capita is greater than US $5000 (constant 2010 US$), b) they engage in distant water fishing, or c) the contribution from Agriculture, Forestry and Fishing to their national GDP (World Bank) is greater than 10%. As written, this exemption might only apply with a transition period, but for the purposes of modeling we assume it to apply indefinitely.</t>
-  </si>
-  <si>
-    <t>Facilitator's text - Overfished [Objective Definition]</t>
-  </si>
-  <si>
-    <t>Facilitator's text - Overfished [Relevant Authorities]</t>
-  </si>
-  <si>
-    <t>Chad on behalf of the Least Developed Countries (LDC) Group</t>
-  </si>
-  <si>
-    <t>Ecuador, Argentina, and Chile</t>
+    <t>OUT/OA</t>
   </si>
 </sst>
 </file>
@@ -2427,9 +2430,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CW45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R44" sqref="R44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2772,7 +2775,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>329</v>
@@ -4222,7 +4225,7 @@
         <v>174</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G20" s="10">
         <v>43803</v>
@@ -4299,7 +4302,7 @@
         <v>174</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G21" s="10">
         <v>43803</v>
@@ -4753,7 +4756,7 @@
         <v>38</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>296</v>
@@ -6719,7 +6722,7 @@
         <v>38</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>287</v>
@@ -6871,19 +6874,19 @@
         <v>423</v>
       </c>
       <c r="N42" s="23" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="O42" s="23" t="s">
         <v>424</v>
       </c>
       <c r="P42" s="23" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="Q42" s="23" t="s">
         <v>425</v>
       </c>
       <c r="R42" s="23" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="S42" s="23" t="s">
         <v>38</v>
@@ -7029,7 +7032,7 @@
         <v>433</v>
       </c>
       <c r="R43" s="23" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="S43" s="23" t="s">
         <v>38</v>
@@ -7121,7 +7124,7 @@
         <v>434</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>196</v>
@@ -7151,19 +7154,19 @@
         <v>423</v>
       </c>
       <c r="N44" s="23" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="O44" s="23" t="s">
         <v>424</v>
       </c>
       <c r="P44" s="23" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="Q44" s="23" t="s">
         <v>438</v>
       </c>
       <c r="R44" s="23" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="S44" s="23" t="s">
         <v>38</v>
@@ -7229,7 +7232,7 @@
         <v>191</v>
       </c>
       <c r="BG44" s="9" t="s">
-        <v>41</v>
+        <v>448</v>
       </c>
       <c r="BI44" s="9">
         <v>5</v>

</xml_diff>

<commit_message>
holding off on Nov text for now
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master_v2.xlsx
+++ b/app/data/wto_proposal_settings_master_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kat/Github/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD53EE4-B77C-DA4E-A81C-6E2EB71FC7F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A557EA77-7EE3-C846-8E40-1C55B9641B69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2473,8 +2473,8 @@
   <dimension ref="A1:CW47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BO43" sqref="BO43"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -7303,7 +7303,7 @@
     </row>
     <row r="45" spans="1:101" ht="297" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>355</v>
@@ -7449,7 +7449,7 @@
     </row>
     <row r="46" spans="1:101" ht="297" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>355</v>

</xml_diff>

<commit_message>
final review of all proposals complete
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master_v2.xlsx
+++ b/app/data/wto_proposal_settings_master_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kat/Github/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A557EA77-7EE3-C846-8E40-1C55B9641B69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2A3236-E8FB-BF41-AC5F-BD0F54E7291D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -784,9 +784,6 @@
     <t>&lt;ol&gt;&lt;li&gt;Final determinations are made by existing RFMO/A vessel lists, by flag, subsidizing, and coastal Member states.&lt;/li&gt;&lt;li&gt;No publically available data exist for most flag and subsidizing Member states, nor for coastal Member states. The possible effects of modeling this proposal is therefore a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about the expected IUU-findings.&lt;/li&gt;&lt;li&gt;No proportionality or the duration of prohibition is considered.&lt;/li&gt;&lt;/ol&gt;</t>
   </si>
   <si>
-    <t>Subsidies granted by LDCs shall be allowed, and subsidies granted by developing countries shall be allowed for fishing in their territorial seas, or for fishing in their EEZs and on the high seas unless any of the following conditions are met for three consecutive years (2016-2018): a) GNI per capita is greater than US $5000 (constant 2010 US$), b) they engage in distant water fishing, or c) the contribution from Agriculture, Forestry and Fishing to their national GDP (World Bank) is greater than 10%.</t>
-  </si>
-  <si>
     <t>This communication presents the current state of the negotiations as they relate to a prohibition on subsidies that contribute to overcapacity and overfishing. A number of different approaches are discussed along with pertaining unresolved questions. This working paper does not contain text suggestions to model, but is included here for reference.</t>
   </si>
   <si>
@@ -803,9 +800,6 @@
   </si>
   <si>
     <t>Subsidies granted by developing and LDC Members shall be allowed for fishing within their own territorial waters.</t>
-  </si>
-  <si>
-    <t>Subsidies granted by LDCs shall be allowed, and subsidies granted by developing countries shall be allowed for fishing in their territorial seas, or for fishing in their EEZs and high seas unless any of the following conditions are met for three consecutive years (2016-2018): a) GNI per capita is greater than US $5000 (constant 2010 US$), b) they engage in distant water fishing, or c) the contribution from Agriculture, Forestry and Fishing to their national GDP (World Bank) is greater than 10%.</t>
   </si>
   <si>
     <t>title_tool_old</t>
@@ -1297,9 +1291,6 @@
   </si>
   <si>
     <t xml:space="preserve">Subsidies granted by developing and LDC Members shall be allowed for small-scale fishing within their own territorial waters. A transition period is considered as an alternative but is not modeled here. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subsidies granted by LDCs shall be allowed, and subsidies granted by all other Members shall be allowed for fishing in their territorial seas. Subsidies granted by developing country Members for fishing in their EEZs and high seas will be allowed unless any of the following conditions are met for three consecutive years (2016-2018): a) GNI per capita is greater than US $5000 (constant 2010 US$), b) they engage in distant water fishing, or c) the contribution from Agriculture, Forestry and Fishing to their national GDP (World Bank) is greater than 10%. A transition period is also considered as an alternative but is not modeled here. If a transition period was employed, we assume that LDCs would enjoy a transition period specifically for them. </t>
   </si>
   <si>
     <t>This proposal excludes subsidies to artisanal fisheries from the prohibitions of Articles 4 and 5. The criteria to consider the exemption is low income, resource poor or livelihood fishing to ensure food security and limited to 12 nautical miles and applicable domestic legislation. To model the possible effects of this proposal, we use the prohibition disciplines proposed in the Chair's text - Consolidated text (Dec 2020) [Relevant Authorities - No cap] (excluding any S&amp;DT).</t>
@@ -1411,9 +1402,6 @@
     <t>Subsidies granted by developing and LDC Members shall be allowed for fishing within their own territorial waters. As written, this exemption might only apply with a transition period, but for the purposes of modeling we assume it to apply indefinitely.</t>
   </si>
   <si>
-    <t>Subsidies granted by LDCs shall be allowed, and subsidies granted by developing countries shall be allowed for fishing in their territorial seas, or for fishing in their EEZs and high seas unless any of the following conditions are met for three consecutive years (2016-2018): a) GNI per capita is greater than US $5000 (constant 2010 US$), b) they engage in distant water fishing, or c) the contribution from Agriculture, Forestry and Fishing to their national GDP (World Bank) is greater than 10%. As written, this exemption might only apply with a transition period, but for the purposes of modeling we assume it to apply indefinitely.</t>
-  </si>
-  <si>
     <t>Facilitator's text - Overfished [Objective Definition]</t>
   </si>
   <si>
@@ -1489,6 +1477,18 @@
   </si>
   <si>
     <t>Subsidies granted by LDCs shall be allowed, and subsidies granted by developing countries shall be allowed for low income, resource-poor, or livelihood fishing in their territorial seas. Developing Members responsible for less than 0.7% of global marine capture production will also be allowed to continue providing subsidies for fishing in their EEZs and in the areas of competence of RFMO/As until they go above that threshold for 3 consecutive years. As written, developing Members may also be allowed to provide subsidies for fishing in their EEZs and in the areas of competence of RFMO/As for a transition period, but this is not modeled.</t>
+  </si>
+  <si>
+    <t>Subsidies granted by LDCs shall be allowed, and subsidies granted by developing countries shall be allowed for fishing in their territorial seas, or for fishing in their EEZs and high seas unless any of the following conditions are met for three consecutive years (2016-2018): a) GNI per capita is greater than US $5000 (constant 2015 US$, World Bank), b) they engage in distant water fishing, or c) the contribution from Agriculture, Forestry and Fishing to their national GDP (World Bank) is greater than 10%. As written, this exemption might only apply with a transition period, but for the purposes of modeling we assume it to apply indefinitely.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subsidies granted by LDCs shall be allowed, and subsidies granted by all other Members shall be allowed for fishing in their territorial seas. Subsidies granted by developing country Members for fishing in their EEZs and high seas will be allowed unless any of the following conditions are met for three consecutive years (2016-2018): a) GNI per capita is greater than US $5000 (constant 2015 US$, World Bank), b) they engage in distant water fishing, or c) the contribution from Agriculture, Forestry and Fishing to their national GDP (World Bank) is greater than 10%. A transition period is also considered as an alternative but is not modeled here. If a transition period was employed, we assume that LDCs would enjoy a transition period specifically for them. </t>
+  </si>
+  <si>
+    <t>Subsidies granted by LDCs shall be allowed, and subsidies granted by developing countries shall be allowed for fishing in their territorial seas, or for fishing in their EEZs and high seas unless any of the following conditions are met for three consecutive years (2016-2018): a) GNI per capita is greater than US $5000 (constant 2015 US$, World Bank), b) they engage in distant water fishing, or c) the contribution from Agriculture, Forestry and Fishing to their national GDP (World Bank) is greater than 10%.</t>
+  </si>
+  <si>
+    <t>Subsidies granted by LDCs shall be allowed, and subsidies granted by developing countries shall be allowed for fishing in their territorial seas, or for fishing in their EEZs and on the high seas unless any of the following conditions are met for three consecutive years (2016-2018): a) GNI per capita is greater than US $5000 (constant 2015 US$, World Bank), b) they engage in distant water fishing, or c) the contribution from Agriculture, Forestry and Fishing to their national GDP (World Bank) is greater than 10%.</t>
   </si>
 </sst>
 </file>
@@ -2472,9 +2472,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CW47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2515,10 +2515,10 @@
         <v>93</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>111</v>
@@ -2817,16 +2817,16 @@
         <v>62</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>178</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G2" s="10">
         <v>43545</v>
@@ -2838,34 +2838,34 @@
         <v>38</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M2" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>248</v>
       </c>
       <c r="O2" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P2" s="23" t="s">
         <v>248</v>
       </c>
       <c r="Q2" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="R2" s="23" t="s">
         <v>248</v>
       </c>
       <c r="S2" s="23" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="T2" s="9"/>
       <c r="U2" s="9"/>
@@ -2983,16 +2983,16 @@
         <v>62</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>166</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G3" s="10">
         <v>43573</v>
@@ -3007,25 +3007,25 @@
         <v>72</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="M3" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N3" s="23" t="s">
         <v>248</v>
       </c>
       <c r="O3" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P3" s="23" t="s">
         <v>248</v>
       </c>
       <c r="Q3" s="23" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="R3" s="23" t="s">
         <v>250</v>
@@ -3060,16 +3060,16 @@
         <v>62</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>164</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G4" s="10">
         <v>43620</v>
@@ -3087,28 +3087,28 @@
         <v>50</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="M4" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N4" s="23" t="s">
         <v>248</v>
       </c>
       <c r="O4" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P4" s="23" t="s">
         <v>248</v>
       </c>
       <c r="Q4" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="R4" s="23" t="s">
         <v>248</v>
       </c>
       <c r="S4" s="23" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="Z4" s="9" t="s">
         <v>153</v>
@@ -3126,10 +3126,10 @@
         <v>211</v>
       </c>
       <c r="CB4" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="CC4" s="9" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="CF4" s="9" t="s">
         <v>201</v>
@@ -3155,16 +3155,16 @@
         <v>80</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>104</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G5" s="10">
         <v>43621</v>
@@ -3179,25 +3179,25 @@
         <v>86</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="L5" s="9" t="s">
         <v>99</v>
       </c>
       <c r="M5" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N5" s="23" t="s">
         <v>248</v>
       </c>
       <c r="O5" s="23" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="P5" s="23" t="s">
         <v>250</v>
       </c>
       <c r="Q5" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="R5" s="23" t="s">
         <v>248</v>
@@ -3232,16 +3232,16 @@
         <v>56</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>101</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G6" s="10">
         <v>43628</v>
@@ -3262,19 +3262,19 @@
         <v>176</v>
       </c>
       <c r="M6" s="23" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="N6" s="23" t="s">
         <v>250</v>
       </c>
       <c r="O6" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P6" s="23" t="s">
         <v>248</v>
       </c>
       <c r="Q6" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="R6" s="23" t="s">
         <v>248</v>
@@ -3312,16 +3312,16 @@
         <v>62</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>102</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G7" s="10">
         <v>43643</v>
@@ -3342,19 +3342,19 @@
         <v>98</v>
       </c>
       <c r="M7" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N7" s="23" t="s">
         <v>248</v>
       </c>
       <c r="O7" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P7" s="23" t="s">
         <v>248</v>
       </c>
       <c r="Q7" s="23" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="R7" s="23" t="s">
         <v>250</v>
@@ -3396,19 +3396,19 @@
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="8" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>167</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G8" s="10">
         <v>43648</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>38</v>
@@ -3420,25 +3420,25 @@
         <v>74</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="M8" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N8" s="23" t="s">
         <v>248</v>
       </c>
       <c r="O8" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P8" s="23" t="s">
         <v>248</v>
       </c>
       <c r="Q8" s="23" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="R8" s="23" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="S8" s="23" t="s">
         <v>38</v>
@@ -3456,7 +3456,7 @@
         <v>191</v>
       </c>
       <c r="BG8" s="9" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="BI8" s="9">
         <v>5</v>
@@ -3488,16 +3488,16 @@
         <v>80</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>103</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G9" s="10">
         <v>43648</v>
@@ -3518,7 +3518,7 @@
         <v>182</v>
       </c>
       <c r="M9" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N9" s="23" t="s">
         <v>248</v>
@@ -3527,10 +3527,10 @@
         <v>252</v>
       </c>
       <c r="P9" s="23" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="Q9" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="R9" s="23" t="s">
         <v>248</v>
@@ -3568,16 +3568,16 @@
         <v>62</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>177</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G10" s="10">
         <v>43657</v>
@@ -3598,25 +3598,25 @@
         <v>223</v>
       </c>
       <c r="M10" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N10" s="23" t="s">
         <v>248</v>
       </c>
       <c r="O10" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P10" s="23" t="s">
         <v>248</v>
       </c>
       <c r="Q10" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="R10" s="23" t="s">
         <v>248</v>
       </c>
       <c r="S10" s="23" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="Z10" s="9" t="s">
         <v>153</v>
@@ -3666,16 +3666,16 @@
         <v>62</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>165</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G11" s="10">
         <v>43684</v>
@@ -3693,22 +3693,22 @@
         <v>73</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="M11" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N11" s="23" t="s">
         <v>248</v>
       </c>
       <c r="O11" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P11" s="23" t="s">
         <v>248</v>
       </c>
       <c r="Q11" s="23" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="R11" s="23" t="s">
         <v>250</v>
@@ -3755,16 +3755,16 @@
         <v>56</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>162</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G12" s="10">
         <v>43718</v>
@@ -3785,19 +3785,19 @@
         <v>97</v>
       </c>
       <c r="M12" s="23" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="N12" s="23" t="s">
         <v>250</v>
       </c>
       <c r="O12" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P12" s="23" t="s">
         <v>248</v>
       </c>
       <c r="Q12" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="R12" s="23" t="s">
         <v>248</v>
@@ -3832,17 +3832,17 @@
         <v>39</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>186</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G13" s="10">
         <v>43759</v>
@@ -3854,7 +3854,7 @@
         <v>39</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="K13" s="9" t="s">
         <v>54</v>
@@ -3863,19 +3863,19 @@
         <v>183</v>
       </c>
       <c r="M13" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N13" s="23" t="s">
         <v>248</v>
       </c>
       <c r="O13" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P13" s="23" t="s">
         <v>248</v>
       </c>
       <c r="Q13" s="23" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="R13" s="23" t="s">
         <v>250</v>
@@ -3913,16 +3913,16 @@
         <v>62</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>226</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G14" s="10">
         <v>43775</v>
@@ -3940,25 +3940,25 @@
         <v>76</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="M14" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N14" s="23" t="s">
         <v>248</v>
       </c>
       <c r="O14" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P14" s="23" t="s">
         <v>248</v>
       </c>
       <c r="Q14" s="23" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="R14" s="23" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="S14" s="23" t="s">
         <v>38</v>
@@ -4002,10 +4002,10 @@
         <v>56</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>240</v>
@@ -4035,16 +4035,16 @@
         <v>253</v>
       </c>
       <c r="N15" s="23" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="O15" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P15" s="23" t="s">
         <v>248</v>
       </c>
       <c r="Q15" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="R15" s="23" t="s">
         <v>248</v>
@@ -4086,13 +4086,13 @@
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="17" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>187</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G16" s="10">
         <v>43801</v>
@@ -4110,16 +4110,16 @@
         <v>96</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="M16" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="O16" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Q16" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:101" ht="112" x14ac:dyDescent="0.2">
@@ -4131,13 +4131,13 @@
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="17" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>188</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G17" s="10">
         <v>43801</v>
@@ -4155,16 +4155,16 @@
         <v>79</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M17" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Q17" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" spans="1:101" ht="56" x14ac:dyDescent="0.2">
@@ -4172,11 +4172,11 @@
         <v>38</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="17" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>189</v>
@@ -4200,16 +4200,16 @@
         <v>88</v>
       </c>
       <c r="L18" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="M18" s="23" t="s">
         <v>257</v>
       </c>
-      <c r="M18" s="23" t="s">
-        <v>258</v>
-      </c>
       <c r="O18" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Q18" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19" spans="1:101" ht="168" x14ac:dyDescent="0.2">
@@ -4220,10 +4220,10 @@
         <v>80</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>174</v>
@@ -4235,7 +4235,7 @@
         <v>43803</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>38</v>
@@ -4261,19 +4261,19 @@
         <v>237</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>174</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="G20" s="10">
         <v>43803</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I20" s="9" t="s">
         <v>38</v>
@@ -4288,19 +4288,19 @@
         <v>224</v>
       </c>
       <c r="M20" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N20" s="23" t="s">
         <v>248</v>
       </c>
       <c r="O20" s="23" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="P20" s="23" t="s">
         <v>250</v>
       </c>
       <c r="Q20" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="R20" s="23" t="s">
         <v>248</v>
@@ -4338,19 +4338,19 @@
         <v>236</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>174</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="G21" s="10">
         <v>43803</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I21" s="9" t="s">
         <v>38</v>
@@ -4365,19 +4365,19 @@
         <v>224</v>
       </c>
       <c r="M21" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N21" s="23" t="s">
         <v>248</v>
       </c>
       <c r="O21" s="23" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="P21" s="23" t="s">
         <v>250</v>
       </c>
       <c r="Q21" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="R21" s="23" t="s">
         <v>248</v>
@@ -4415,13 +4415,13 @@
         <v>217</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>106</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G22" s="10">
         <v>43843</v>
@@ -4442,19 +4442,19 @@
         <v>180</v>
       </c>
       <c r="M22" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N22" s="23" t="s">
         <v>248</v>
       </c>
       <c r="O22" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P22" s="23" t="s">
         <v>248</v>
       </c>
       <c r="Q22" s="23" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="R22" s="23" t="s">
         <v>250</v>
@@ -4501,16 +4501,16 @@
         <v>56</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>100</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G23" s="10">
         <v>43865</v>
@@ -4528,22 +4528,22 @@
         <v>92</v>
       </c>
       <c r="L23" s="9" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M23" s="23" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N23" s="23" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="O23" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P23" s="23" t="s">
         <v>248</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="R23" s="23" t="s">
         <v>248</v>
@@ -4608,16 +4608,16 @@
         <v>62</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>168</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G24" s="10">
         <v>43865</v>
@@ -4638,19 +4638,19 @@
         <v>184</v>
       </c>
       <c r="M24" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N24" s="23" t="s">
         <v>248</v>
       </c>
       <c r="O24" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P24" s="23" t="s">
         <v>248</v>
       </c>
       <c r="Q24" s="23" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="R24" s="23" t="s">
         <v>212</v>
@@ -4668,7 +4668,7 @@
         <v>43</v>
       </c>
       <c r="BF24" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="BM24" s="9" t="s">
         <v>160</v>
@@ -4697,16 +4697,16 @@
         <v>62</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>222</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G25" s="14">
         <v>43890</v>
@@ -4724,28 +4724,28 @@
         <v>220</v>
       </c>
       <c r="L25" s="9" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="M25" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N25" s="24" t="s">
         <v>248</v>
       </c>
       <c r="O25" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P25" s="24" t="s">
         <v>248</v>
       </c>
       <c r="Q25" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="R25" s="24" t="s">
         <v>248</v>
       </c>
       <c r="S25" s="24" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="Z25" s="9" t="s">
         <v>153</v>
@@ -4774,19 +4774,19 @@
         <v>39</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>163</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G26" s="14">
         <v>43896</v>
@@ -4798,31 +4798,31 @@
         <v>38</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>185</v>
       </c>
       <c r="M26" s="24" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N26" s="24" t="s">
         <v>250</v>
       </c>
       <c r="O26" s="24" t="s">
+        <v>374</v>
+      </c>
+      <c r="P26" s="24" t="s">
+        <v>375</v>
+      </c>
+      <c r="Q26" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="P26" s="24" t="s">
+      <c r="R26" s="24" t="s">
         <v>377</v>
-      </c>
-      <c r="Q26" s="24" t="s">
-        <v>378</v>
-      </c>
-      <c r="R26" s="24" t="s">
-        <v>379</v>
       </c>
       <c r="S26" s="24" t="s">
         <v>38</v>
@@ -4971,19 +4971,19 @@
         <v>39</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>110</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G27" s="10">
         <v>43896</v>
@@ -5001,25 +5001,25 @@
         <v>90</v>
       </c>
       <c r="L27" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="M27" s="24" t="s">
+        <v>366</v>
+      </c>
+      <c r="N27" s="23" t="s">
+        <v>379</v>
+      </c>
+      <c r="O27" s="24" t="s">
+        <v>374</v>
+      </c>
+      <c r="P27" s="23" t="s">
         <v>380</v>
       </c>
-      <c r="M27" s="24" t="s">
-        <v>368</v>
-      </c>
-      <c r="N27" s="23" t="s">
-        <v>381</v>
-      </c>
-      <c r="O27" s="24" t="s">
+      <c r="Q27" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="P27" s="23" t="s">
-        <v>382</v>
-      </c>
-      <c r="Q27" s="24" t="s">
-        <v>378</v>
-      </c>
       <c r="R27" s="23" t="s">
-        <v>254</v>
+        <v>462</v>
       </c>
       <c r="S27" s="23" t="s">
         <v>38</v>
@@ -5126,22 +5126,22 @@
         <v>62</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>222</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G28" s="14">
         <v>44110</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>38</v>
@@ -5150,31 +5150,31 @@
         <v>219</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="M28" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N28" s="24" t="s">
         <v>248</v>
       </c>
       <c r="O28" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P28" s="24" t="s">
         <v>248</v>
       </c>
       <c r="Q28" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="R28" s="24" t="s">
         <v>248</v>
       </c>
       <c r="S28" s="24" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="Z28" s="9" t="s">
         <v>153</v>
@@ -5203,25 +5203,25 @@
         <v>39</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>196</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G29" s="10">
         <v>44183</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I29" s="8" t="s">
         <v>38</v>
@@ -5230,7 +5230,7 @@
         <v>195</v>
       </c>
       <c r="K29" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L29" s="9" t="s">
         <v>242</v>
@@ -5251,25 +5251,25 @@
         <v>221</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>239</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>196</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G30" s="10">
         <v>44183</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I30" s="8" t="s">
         <v>38</v>
@@ -5278,28 +5278,28 @@
         <v>195</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L30" s="9" t="s">
         <v>242</v>
       </c>
       <c r="M30" s="23" t="s">
+        <v>389</v>
+      </c>
+      <c r="N30" s="23" t="s">
+        <v>390</v>
+      </c>
+      <c r="O30" s="23" t="s">
+        <v>363</v>
+      </c>
+      <c r="P30" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q30" s="23" t="s">
         <v>391</v>
       </c>
-      <c r="N30" s="23" t="s">
-        <v>392</v>
-      </c>
-      <c r="O30" s="23" t="s">
-        <v>365</v>
-      </c>
-      <c r="P30" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q30" s="23" t="s">
-        <v>393</v>
-      </c>
       <c r="R30" s="23" t="s">
-        <v>261</v>
+        <v>461</v>
       </c>
       <c r="S30" s="23" t="s">
         <v>38</v>
@@ -5397,25 +5397,25 @@
         <v>221</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>238</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>196</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="G31" s="10">
         <v>44183</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I31" s="8" t="s">
         <v>38</v>
@@ -5424,28 +5424,28 @@
         <v>195</v>
       </c>
       <c r="K31" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L31" s="9" t="s">
         <v>242</v>
       </c>
       <c r="M31" s="23" t="s">
+        <v>389</v>
+      </c>
+      <c r="N31" s="23" t="s">
+        <v>390</v>
+      </c>
+      <c r="O31" s="23" t="s">
+        <v>364</v>
+      </c>
+      <c r="P31" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q31" s="23" t="s">
         <v>391</v>
       </c>
-      <c r="N31" s="23" t="s">
-        <v>392</v>
-      </c>
-      <c r="O31" s="23" t="s">
-        <v>366</v>
-      </c>
-      <c r="P31" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q31" s="23" t="s">
-        <v>393</v>
-      </c>
       <c r="R31" s="23" t="s">
-        <v>261</v>
+        <v>461</v>
       </c>
       <c r="S31" s="23" t="s">
         <v>38</v>
@@ -5543,25 +5543,25 @@
         <v>221</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>234</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>196</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="G32" s="10">
         <v>44183</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I32" s="8" t="s">
         <v>38</v>
@@ -5570,31 +5570,31 @@
         <v>195</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L32" s="9" t="s">
         <v>242</v>
       </c>
       <c r="M32" s="23" t="s">
+        <v>389</v>
+      </c>
+      <c r="N32" s="23" t="s">
+        <v>390</v>
+      </c>
+      <c r="O32" s="23" t="s">
+        <v>363</v>
+      </c>
+      <c r="P32" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q32" s="23" t="s">
         <v>391</v>
       </c>
-      <c r="N32" s="23" t="s">
-        <v>392</v>
-      </c>
-      <c r="O32" s="23" t="s">
-        <v>365</v>
-      </c>
-      <c r="P32" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q32" s="23" t="s">
-        <v>393</v>
-      </c>
       <c r="R32" s="23" t="s">
-        <v>261</v>
+        <v>461</v>
       </c>
       <c r="S32" s="23" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="T32" s="9" t="s">
         <v>197</v>
@@ -5707,25 +5707,25 @@
         <v>221</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C33" s="20" t="s">
         <v>235</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>196</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="G33" s="10">
         <v>44183</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="I33" s="8" t="s">
         <v>38</v>
@@ -5734,31 +5734,31 @@
         <v>195</v>
       </c>
       <c r="K33" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L33" s="9" t="s">
         <v>242</v>
       </c>
       <c r="M33" s="23" t="s">
+        <v>389</v>
+      </c>
+      <c r="N33" s="23" t="s">
+        <v>390</v>
+      </c>
+      <c r="O33" s="23" t="s">
+        <v>364</v>
+      </c>
+      <c r="P33" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q33" s="23" t="s">
         <v>391</v>
       </c>
-      <c r="N33" s="23" t="s">
-        <v>392</v>
-      </c>
-      <c r="O33" s="23" t="s">
-        <v>366</v>
-      </c>
-      <c r="P33" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q33" s="23" t="s">
-        <v>393</v>
-      </c>
       <c r="R33" s="23" t="s">
-        <v>261</v>
+        <v>461</v>
       </c>
       <c r="S33" s="23" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="T33" s="9" t="s">
         <v>197</v>
@@ -5871,25 +5871,25 @@
         <v>221</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C34" s="20" t="s">
         <v>232</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E34" s="11" t="s">
         <v>196</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G34" s="10">
         <v>44183</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>38</v>
@@ -5898,31 +5898,31 @@
         <v>195</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L34" s="9" t="s">
         <v>242</v>
       </c>
       <c r="M34" s="23" t="s">
+        <v>389</v>
+      </c>
+      <c r="N34" s="23" t="s">
+        <v>390</v>
+      </c>
+      <c r="O34" s="23" t="s">
+        <v>363</v>
+      </c>
+      <c r="P34" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q34" s="23" t="s">
         <v>391</v>
       </c>
-      <c r="N34" s="23" t="s">
-        <v>392</v>
-      </c>
-      <c r="O34" s="23" t="s">
-        <v>365</v>
-      </c>
-      <c r="P34" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q34" s="23" t="s">
-        <v>393</v>
-      </c>
       <c r="R34" s="23" t="s">
-        <v>261</v>
+        <v>461</v>
       </c>
       <c r="S34" s="23" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="T34" s="9" t="s">
         <v>197</v>
@@ -6014,25 +6014,25 @@
         <v>221</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C35" s="20" t="s">
         <v>233</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E35" s="11" t="s">
         <v>196</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G35" s="10">
         <v>44183</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="I35" s="8" t="s">
         <v>38</v>
@@ -6041,31 +6041,31 @@
         <v>195</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L35" s="9" t="s">
         <v>242</v>
       </c>
       <c r="M35" s="23" t="s">
+        <v>389</v>
+      </c>
+      <c r="N35" s="23" t="s">
+        <v>390</v>
+      </c>
+      <c r="O35" s="23" t="s">
+        <v>364</v>
+      </c>
+      <c r="P35" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q35" s="23" t="s">
         <v>391</v>
       </c>
-      <c r="N35" s="23" t="s">
-        <v>392</v>
-      </c>
-      <c r="O35" s="23" t="s">
-        <v>366</v>
-      </c>
-      <c r="P35" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q35" s="23" t="s">
-        <v>393</v>
-      </c>
       <c r="R35" s="23" t="s">
-        <v>261</v>
+        <v>461</v>
       </c>
       <c r="S35" s="23" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="T35" s="9" t="s">
         <v>197</v>
@@ -6157,25 +6157,25 @@
         <v>221</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C36" s="20" t="s">
         <v>231</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>196</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G36" s="10">
         <v>44183</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I36" s="8" t="s">
         <v>38</v>
@@ -6184,31 +6184,31 @@
         <v>195</v>
       </c>
       <c r="K36" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L36" s="9" t="s">
         <v>242</v>
       </c>
       <c r="M36" s="23" t="s">
+        <v>389</v>
+      </c>
+      <c r="N36" s="23" t="s">
+        <v>390</v>
+      </c>
+      <c r="O36" s="23" t="s">
+        <v>363</v>
+      </c>
+      <c r="P36" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q36" s="23" t="s">
         <v>391</v>
       </c>
-      <c r="N36" s="23" t="s">
-        <v>392</v>
-      </c>
-      <c r="O36" s="23" t="s">
-        <v>365</v>
-      </c>
-      <c r="P36" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q36" s="23" t="s">
-        <v>393</v>
-      </c>
       <c r="R36" s="23" t="s">
-        <v>261</v>
+        <v>461</v>
       </c>
       <c r="S36" s="23" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="T36" s="9" t="s">
         <v>197</v>
@@ -6301,25 +6301,25 @@
         <v>221</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C37" s="20" t="s">
         <v>230</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>196</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G37" s="10">
         <v>44183</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="I37" s="8" t="s">
         <v>38</v>
@@ -6328,31 +6328,31 @@
         <v>195</v>
       </c>
       <c r="K37" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L37" s="9" t="s">
         <v>242</v>
       </c>
       <c r="M37" s="23" t="s">
+        <v>389</v>
+      </c>
+      <c r="N37" s="23" t="s">
+        <v>390</v>
+      </c>
+      <c r="O37" s="23" t="s">
+        <v>364</v>
+      </c>
+      <c r="P37" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q37" s="23" t="s">
         <v>391</v>
       </c>
-      <c r="N37" s="23" t="s">
-        <v>392</v>
-      </c>
-      <c r="O37" s="23" t="s">
-        <v>366</v>
-      </c>
-      <c r="P37" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q37" s="23" t="s">
-        <v>393</v>
-      </c>
       <c r="R37" s="23" t="s">
-        <v>261</v>
+        <v>461</v>
       </c>
       <c r="S37" s="23" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="T37" s="9" t="s">
         <v>197</v>
@@ -6445,25 +6445,25 @@
         <v>221</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C38" s="20" t="s">
         <v>228</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E38" s="11" t="s">
         <v>196</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="G38" s="10">
         <v>44183</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I38" s="8" t="s">
         <v>38</v>
@@ -6472,31 +6472,31 @@
         <v>195</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L38" s="9" t="s">
         <v>242</v>
       </c>
       <c r="M38" s="23" t="s">
+        <v>389</v>
+      </c>
+      <c r="N38" s="23" t="s">
+        <v>390</v>
+      </c>
+      <c r="O38" s="23" t="s">
+        <v>363</v>
+      </c>
+      <c r="P38" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q38" s="23" t="s">
         <v>391</v>
       </c>
-      <c r="N38" s="23" t="s">
-        <v>392</v>
-      </c>
-      <c r="O38" s="23" t="s">
-        <v>365</v>
-      </c>
-      <c r="P38" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q38" s="23" t="s">
-        <v>393</v>
-      </c>
       <c r="R38" s="23" t="s">
-        <v>261</v>
+        <v>461</v>
       </c>
       <c r="S38" s="24" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="T38" s="9" t="s">
         <v>197</v>
@@ -6570,25 +6570,25 @@
         <v>221</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C39" s="20" t="s">
         <v>229</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E39" s="11" t="s">
         <v>196</v>
       </c>
       <c r="F39" s="29" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="G39" s="10">
         <v>44183</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="I39" s="8" t="s">
         <v>38</v>
@@ -6597,31 +6597,31 @@
         <v>195</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L39" s="9" t="s">
         <v>242</v>
       </c>
       <c r="M39" s="23" t="s">
+        <v>389</v>
+      </c>
+      <c r="N39" s="23" t="s">
+        <v>390</v>
+      </c>
+      <c r="O39" s="23" t="s">
+        <v>364</v>
+      </c>
+      <c r="P39" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q39" s="23" t="s">
         <v>391</v>
       </c>
-      <c r="N39" s="23" t="s">
-        <v>392</v>
-      </c>
-      <c r="O39" s="23" t="s">
-        <v>366</v>
-      </c>
-      <c r="P39" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q39" s="23" t="s">
-        <v>393</v>
-      </c>
       <c r="R39" s="23" t="s">
-        <v>261</v>
+        <v>461</v>
       </c>
       <c r="S39" s="24" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="T39" s="9" t="s">
         <v>197</v>
@@ -6695,44 +6695,44 @@
         <v>38</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C40" s="20"/>
       <c r="D40" s="8" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G40" s="14">
         <v>44246</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>38</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="M40" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="O40" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Q40" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="41" spans="1:101" ht="297" customHeight="1" x14ac:dyDescent="0.2">
@@ -6740,55 +6740,55 @@
         <v>39</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G41" s="14">
         <v>44249</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I41" s="4" t="s">
         <v>38</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="M41" s="23" t="s">
+        <v>389</v>
+      </c>
+      <c r="N41" s="23" t="s">
+        <v>416</v>
+      </c>
+      <c r="O41" s="23" t="s">
+        <v>364</v>
+      </c>
+      <c r="P41" s="23" t="s">
+        <v>303</v>
+      </c>
+      <c r="Q41" s="23" t="s">
         <v>391</v>
       </c>
-      <c r="N41" s="23" t="s">
-        <v>418</v>
-      </c>
-      <c r="O41" s="23" t="s">
-        <v>366</v>
-      </c>
-      <c r="P41" s="23" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q41" s="23" t="s">
-        <v>393</v>
-      </c>
       <c r="R41" s="23" t="s">
-        <v>419</v>
+        <v>460</v>
       </c>
       <c r="S41" s="23" t="s">
         <v>38</v>
@@ -6880,25 +6880,25 @@
         <v>39</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="E42" s="11" t="s">
         <v>196</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="G42" s="10">
         <v>44327</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="I42" s="8" t="s">
         <v>39</v>
@@ -6907,34 +6907,34 @@
         <v>195</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="L42" s="9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="M42" s="23" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="N42" s="23" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="O42" s="23" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="P42" s="23" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="Q42" s="23" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="R42" s="23" t="s">
-        <v>442</v>
+        <v>459</v>
       </c>
       <c r="S42" s="23" t="s">
         <v>38</v>
       </c>
       <c r="T42" s="9" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="U42" s="9" t="s">
         <v>153</v>
@@ -7026,25 +7026,25 @@
         <v>39</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>196</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="G43" s="10">
         <v>44327</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="I43" s="8" t="s">
         <v>39</v>
@@ -7053,34 +7053,34 @@
         <v>195</v>
       </c>
       <c r="K43" s="9" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="L43" s="9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="M43" s="23" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="N43" s="23" t="s">
         <v>250</v>
       </c>
       <c r="O43" s="23" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="P43" s="23" t="s">
         <v>250</v>
       </c>
       <c r="Q43" s="23" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="R43" s="23" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="S43" s="23" t="s">
         <v>38</v>
       </c>
       <c r="T43" s="9" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="U43" s="9" t="s">
         <v>160</v>
@@ -7160,25 +7160,25 @@
         <v>39</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>196</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="G44" s="10">
         <v>44327</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="I44" s="8" t="s">
         <v>39</v>
@@ -7187,34 +7187,34 @@
         <v>195</v>
       </c>
       <c r="K44" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="L44" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="M44" s="23" t="s">
+        <v>420</v>
+      </c>
+      <c r="N44" s="23" t="s">
         <v>437</v>
       </c>
-      <c r="L44" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="M44" s="23" t="s">
-        <v>423</v>
-      </c>
-      <c r="N44" s="23" t="s">
-        <v>440</v>
-      </c>
       <c r="O44" s="23" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="P44" s="23" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="Q44" s="23" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="R44" s="23" t="s">
-        <v>442</v>
+        <v>459</v>
       </c>
       <c r="S44" s="23" t="s">
         <v>38</v>
       </c>
       <c r="T44" s="9" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="U44" s="9" t="s">
         <v>153</v>
@@ -7274,7 +7274,7 @@
         <v>191</v>
       </c>
       <c r="BG44" s="9" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="BI44" s="9">
         <v>5</v>
@@ -7306,61 +7306,61 @@
         <v>38</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="G45" s="10">
         <v>44524</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="I45" s="8" t="s">
         <v>39</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="K45" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="L45" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="M45" s="23" t="s">
+        <v>420</v>
+      </c>
+      <c r="N45" s="23" t="s">
+        <v>451</v>
+      </c>
+      <c r="O45" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="L45" s="9" t="s">
-        <v>454</v>
-      </c>
-      <c r="M45" s="23" t="s">
-        <v>423</v>
-      </c>
-      <c r="N45" s="23" t="s">
-        <v>455</v>
-      </c>
-      <c r="O45" s="23" t="s">
-        <v>456</v>
-      </c>
       <c r="P45" s="23" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="Q45" s="23" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="R45" s="23" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="S45" s="23" t="s">
         <v>38</v>
       </c>
       <c r="T45" s="9" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="U45" s="9" t="s">
         <v>153</v>
@@ -7452,61 +7452,61 @@
         <v>38</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="G46" s="10">
         <v>44524</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="I46" s="8" t="s">
         <v>39</v>
       </c>
       <c r="J46" s="9" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="K46" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="L46" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="M46" s="23" t="s">
+        <v>420</v>
+      </c>
+      <c r="N46" s="23" t="s">
+        <v>451</v>
+      </c>
+      <c r="O46" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="L46" s="9" t="s">
-        <v>454</v>
-      </c>
-      <c r="M46" s="23" t="s">
-        <v>423</v>
-      </c>
-      <c r="N46" s="23" t="s">
-        <v>455</v>
-      </c>
-      <c r="O46" s="23" t="s">
-        <v>456</v>
-      </c>
       <c r="P46" s="23" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="Q46" s="23" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="R46" s="23" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="S46" s="23" t="s">
         <v>38</v>
       </c>
       <c r="T46" s="9" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="U46" s="9" t="s">
         <v>153</v>
@@ -7566,7 +7566,7 @@
         <v>191</v>
       </c>
       <c r="BG46" s="9" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="BI46" s="9">
         <v>5</v>

</xml_diff>